<commit_message>
created transformations in 3d space
filtered out z coordinates that are below 0
</commit_message>
<xml_diff>
--- a/VisionModel/output/predicted_trajectoriesX.xlsx
+++ b/VisionModel/output/predicted_trajectoriesX.xlsx
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1778.057076217292</v>
+        <v>1486.023634431477</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>0.03333333333333333</v>
       </c>
       <c r="B3" t="n">
-        <v>2409.874878525266</v>
+        <v>2298.135986457459</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>0.06666666666666667</v>
       </c>
       <c r="B4" t="n">
-        <v>3254.910141977524</v>
+        <v>3139.354815071962</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>0.1</v>
       </c>
       <c r="B5" t="n">
-        <v>4007.149448471991</v>
+        <v>3932.878714179342</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>0.1333333333333333</v>
       </c>
       <c r="B6" t="n">
-        <v>4684.334870199338</v>
+        <v>4565.23899803468</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>0.1666666666666667</v>
       </c>
       <c r="B7" t="n">
-        <v>5247.702959446491</v>
+        <v>5056.847638022701</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>0.2</v>
       </c>
       <c r="B8" t="n">
-        <v>5611.828717742312</v>
+        <v>5513.233265149313</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>0.2333333333333333</v>
       </c>
       <c r="B9" t="n">
-        <v>6087.604166346948</v>
+        <v>6063.281889589232</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>0.2666666666666667</v>
       </c>
       <c r="B10" t="n">
-        <v>6483.88189574066</v>
+        <v>6446.602767067534</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>0.3</v>
       </c>
       <c r="B11" t="n">
-        <v>6724.327917529955</v>
+        <v>6812.148783421399</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="B12" t="n">
-        <v>7266.979975408748</v>
+        <v>7149.665591886473</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>0.3666666666666666</v>
       </c>
       <c r="B13" t="n">
-        <v>7555.656221323939</v>
+        <v>7451.723706815204</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>0.4</v>
       </c>
       <c r="B14" t="n">
-        <v>7894.417582497334</v>
+        <v>7774.856869573544</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>0.4333333333333333</v>
       </c>
       <c r="B15" t="n">
-        <v>8122.253148753268</v>
+        <v>8127.005400009524</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>0.4666666666666667</v>
       </c>
       <c r="B16" t="n">
-        <v>8438.704344040732</v>
+        <v>8445.843967366611</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>0.5</v>
       </c>
       <c r="B17" t="n">
-        <v>8729.109390175639</v>
+        <v>8717.227856540376</v>
       </c>
     </row>
     <row r="18">
@@ -578,7 +578,7 @@
         <v>0.5333333333333333</v>
       </c>
       <c r="B18" t="n">
-        <v>8888.564641891891</v>
+        <v>8889.082856292411</v>
       </c>
     </row>
     <row r="19">
@@ -586,7 +586,7 @@
         <v>0.5666666666666667</v>
       </c>
       <c r="B19" t="n">
-        <v>9078.775689791411</v>
+        <v>9100.810779565025</v>
       </c>
     </row>
     <row r="20">
@@ -594,7 +594,7 @@
         <v>0.6</v>
       </c>
       <c r="B20" t="n">
-        <v>9594.230000559099</v>
+        <v>9542.510798792076</v>
       </c>
     </row>
     <row r="21">
@@ -602,7 +602,7 @@
         <v>0.6333333333333333</v>
       </c>
       <c r="B21" t="n">
-        <v>9674.446987474204</v>
+        <v>9699.766527666708</v>
       </c>
     </row>
     <row r="22">
@@ -610,7 +610,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>9866.526380062289</v>
+        <v>9927.335242497451</v>
       </c>
     </row>
     <row r="23">
@@ -618,7 +618,7 @@
         <v>0.7</v>
       </c>
       <c r="B23" t="n">
-        <v>9983.479091734813</v>
+        <v>10080.73034756769</v>
       </c>
     </row>
     <row r="24">
@@ -626,7 +626,7 @@
         <v>0.7333333333333333</v>
       </c>
       <c r="B24" t="n">
-        <v>10397.57054671569</v>
+        <v>10379.20822118833</v>
       </c>
     </row>
     <row r="25">
@@ -634,7 +634,7 @@
         <v>0.7666666666666666</v>
       </c>
       <c r="B25" t="n">
-        <v>10596.84244310312</v>
+        <v>10567.4328674492</v>
       </c>
     </row>
     <row r="26">
@@ -642,7 +642,7 @@
         <v>0.8</v>
       </c>
       <c r="B26" t="n">
-        <v>10710.26496171905</v>
+        <v>10689.34202809058</v>
       </c>
     </row>
     <row r="27">
@@ -650,7 +650,7 @@
         <v>0.8333333333333334</v>
       </c>
       <c r="B27" t="n">
-        <v>10900.80588791535</v>
+        <v>10874.44348788996</v>
       </c>
     </row>
     <row r="28">
@@ -658,7 +658,7 @@
         <v>0.8666666666666667</v>
       </c>
       <c r="B28" t="n">
-        <v>11020.22197989293</v>
+        <v>10981.21679639662</v>
       </c>
     </row>
     <row r="29">
@@ -666,7 +666,7 @@
         <v>0.9</v>
       </c>
       <c r="B29" t="n">
-        <v>11195.19758457124</v>
+        <v>11193.3142242274</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +674,7 @@
         <v>0.9333333333333333</v>
       </c>
       <c r="B30" t="n">
-        <v>11323.47241928449</v>
+        <v>11323.58291949659</v>
       </c>
     </row>
     <row r="31">
@@ -682,7 +682,7 @@
         <v>0.9666666666666667</v>
       </c>
       <c r="B31" t="n">
-        <v>11422.80017156268</v>
+        <v>11468.94226962042</v>
       </c>
     </row>
     <row r="32">
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>11666.77520311872</v>
+        <v>11779.70520856214</v>
       </c>
     </row>
     <row r="33">
@@ -698,7 +698,7 @@
         <v>1.033333333333333</v>
       </c>
       <c r="B33" t="n">
-        <v>11813.39475370939</v>
+        <v>11864.82703546343</v>
       </c>
     </row>
     <row r="34">
@@ -706,7 +706,7 @@
         <v>1.066666666666667</v>
       </c>
       <c r="B34" t="n">
-        <v>11999.2206345932</v>
+        <v>12018.08718247714</v>
       </c>
     </row>
     <row r="35">
@@ -714,7 +714,7 @@
         <v>1.1</v>
       </c>
       <c r="B35" t="n">
-        <v>12087.90140880381</v>
+        <v>12172.32478077167</v>
       </c>
     </row>
     <row r="36">
@@ -722,7 +722,7 @@
         <v>1.133333333333333</v>
       </c>
       <c r="B36" t="n">
-        <v>12252.1400621099</v>
+        <v>12245.43284544658</v>
       </c>
     </row>
     <row r="37">
@@ -730,7 +730,7 @@
         <v>1.166666666666667</v>
       </c>
       <c r="B37" t="n">
-        <v>12322.07406377938</v>
+        <v>12325.09708835992</v>
       </c>
     </row>
     <row r="38">
@@ -738,7 +738,7 @@
         <v>1.2</v>
       </c>
       <c r="B38" t="n">
-        <v>12552.38827565591</v>
+        <v>12508.08077212547</v>
       </c>
     </row>
     <row r="39">
@@ -746,7 +746,7 @@
         <v>1.233333333333333</v>
       </c>
       <c r="B39" t="n">
-        <v>12623.42867165452</v>
+        <v>12635.42560401157</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +754,7 @@
         <v>1.266666666666667</v>
       </c>
       <c r="B40" t="n">
-        <v>12859.86104222549</v>
+        <v>12760.11872401384</v>
       </c>
     </row>
     <row r="41">
@@ -762,7 +762,7 @@
         <v>1.3</v>
       </c>
       <c r="B41" t="n">
-        <v>12986.563075041</v>
+        <v>12848.50243680028</v>
       </c>
     </row>
     <row r="42">
@@ -770,7 +770,7 @@
         <v>1.333333333333333</v>
       </c>
       <c r="B42" t="n">
-        <v>13113.67219393253</v>
+        <v>12981.51286316499</v>
       </c>
     </row>
     <row r="43">
@@ -778,7 +778,7 @@
         <v>1.366666666666667</v>
       </c>
       <c r="B43" t="n">
-        <v>13167.20370706843</v>
+        <v>13054.52222273246</v>
       </c>
     </row>
     <row r="44">
@@ -786,7 +786,7 @@
         <v>1.4</v>
       </c>
       <c r="B44" t="n">
-        <v>13260.96743559498</v>
+        <v>13151.68102437822</v>
       </c>
     </row>
     <row r="45">
@@ -794,7 +794,7 @@
         <v>1.433333333333333</v>
       </c>
       <c r="B45" t="n">
-        <v>13367.27830947661</v>
+        <v>13287.58764252546</v>
       </c>
     </row>
     <row r="46">
@@ -802,7 +802,7 @@
         <v>1.466666666666667</v>
       </c>
       <c r="B46" t="n">
-        <v>13455.8328659066</v>
+        <v>13362.2976451646</v>
       </c>
     </row>
     <row r="47">
@@ -810,7 +810,7 @@
         <v>1.5</v>
       </c>
       <c r="B47" t="n">
-        <v>13592.40898719582</v>
+        <v>13490.48414440517</v>
       </c>
     </row>
     <row r="48">
@@ -818,7 +818,7 @@
         <v>1.533333333333333</v>
       </c>
       <c r="B48" t="n">
-        <v>13728.19996878413</v>
+        <v>13593.58868484142</v>
       </c>
     </row>
     <row r="49">
@@ -826,7 +826,7 @@
         <v>1.566666666666667</v>
       </c>
       <c r="B49" t="n">
-        <v>13732.14285249094</v>
+        <v>13596.94102936735</v>
       </c>
     </row>
     <row r="50">
@@ -834,7 +834,7 @@
         <v>1.6</v>
       </c>
       <c r="B50" t="n">
-        <v>13746.17957652823</v>
+        <v>13669.34852991616</v>
       </c>
     </row>
     <row r="51">
@@ -842,7 +842,7 @@
         <v>1.633333333333333</v>
       </c>
       <c r="B51" t="n">
-        <v>13856.03159825715</v>
+        <v>13776.84786942862</v>
       </c>
     </row>
     <row r="52">
@@ -850,7 +850,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="B52" t="n">
-        <v>13938.4531294855</v>
+        <v>13848.21150601052</v>
       </c>
     </row>
     <row r="53">
@@ -858,7 +858,7 @@
         <v>1.7</v>
       </c>
       <c r="B53" t="n">
-        <v>14030.97478802515</v>
+        <v>13919.58437113316</v>
       </c>
     </row>
     <row r="54">
@@ -866,7 +866,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="B54" t="n">
-        <v>14108.86847882094</v>
+        <v>13963.38835751431</v>
       </c>
     </row>
     <row r="55">
@@ -874,7 +874,7 @@
         <v>1.766666666666667</v>
       </c>
       <c r="B55" t="n">
-        <v>14265.70785737322</v>
+        <v>14110.50446643876</v>
       </c>
     </row>
     <row r="56">
@@ -882,7 +882,7 @@
         <v>1.8</v>
       </c>
       <c r="B56" t="n">
-        <v>14217.75239397424</v>
+        <v>14100.85439618242</v>
       </c>
     </row>
     <row r="57">
@@ -890,7 +890,7 @@
         <v>1.833333333333333</v>
       </c>
       <c r="B57" t="n">
-        <v>14285.94694507579</v>
+        <v>14189.26885625105</v>
       </c>
     </row>
     <row r="58">
@@ -898,7 +898,7 @@
         <v>1.866666666666667</v>
       </c>
       <c r="B58" t="n">
-        <v>14297.93185812813</v>
+        <v>14193.50717267355</v>
       </c>
     </row>
     <row r="59">
@@ -906,7 +906,7 @@
         <v>1.9</v>
       </c>
       <c r="B59" t="n">
-        <v>14297.48392724881</v>
+        <v>14238.93986774932</v>
       </c>
     </row>
     <row r="60">
@@ -914,7 +914,7 @@
         <v>1.933333333333333</v>
       </c>
       <c r="B60" t="n">
-        <v>14456.01892018937</v>
+        <v>14387.6725881826</v>
       </c>
     </row>
     <row r="61">
@@ -922,7 +922,7 @@
         <v>1.966666666666667</v>
       </c>
       <c r="B61" t="n">
-        <v>14476.54983133553</v>
+        <v>14394.71257736065</v>
       </c>
     </row>
     <row r="62">
@@ -930,7 +930,7 @@
         <v>2</v>
       </c>
       <c r="B62" t="n">
-        <v>14530.35412783211</v>
+        <v>14413.16179364517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented findStart but discovered problems with 3D transform
</commit_message>
<xml_diff>
--- a/VisionModel/output/predicted_trajectoriesX.xlsx
+++ b/VisionModel/output/predicted_trajectoriesX.xlsx
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1486.023634431477</v>
+        <v>2896.016791289029</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>0.03333333333333333</v>
       </c>
       <c r="B3" t="n">
-        <v>2298.135986457459</v>
+        <v>3927.658649050765</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>0.06666666666666667</v>
       </c>
       <c r="B4" t="n">
-        <v>3139.354815071962</v>
+        <v>4534.029129713806</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>0.1</v>
       </c>
       <c r="B5" t="n">
-        <v>3932.878714179342</v>
+        <v>5421.269083827</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>0.1333333333333333</v>
       </c>
       <c r="B6" t="n">
-        <v>4565.23899803468</v>
+        <v>6030.559498840906</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>0.1666666666666667</v>
       </c>
       <c r="B7" t="n">
-        <v>5056.847638022701</v>
+        <v>6525.100025618548</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>0.2</v>
       </c>
       <c r="B8" t="n">
-        <v>5513.233265149313</v>
+        <v>6952.981220056842</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>0.2333333333333333</v>
       </c>
       <c r="B9" t="n">
-        <v>6063.281889589232</v>
+        <v>7484.473598119846</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>0.2666666666666667</v>
       </c>
       <c r="B10" t="n">
-        <v>6446.602767067534</v>
+        <v>7843.293491568781</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>0.3</v>
       </c>
       <c r="B11" t="n">
-        <v>6812.148783421399</v>
+        <v>8290.187337687727</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="B12" t="n">
-        <v>7149.665591886473</v>
+        <v>8685.730032810463</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>0.3666666666666666</v>
       </c>
       <c r="B13" t="n">
-        <v>7451.723706815204</v>
+        <v>9001.70057840767</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>0.4</v>
       </c>
       <c r="B14" t="n">
-        <v>7774.856869573544</v>
+        <v>9226.559212791988</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>0.4333333333333333</v>
       </c>
       <c r="B15" t="n">
-        <v>8127.005400009524</v>
+        <v>9552.597441704291</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>0.4666666666666667</v>
       </c>
       <c r="B16" t="n">
-        <v>8445.843967366611</v>
+        <v>9856.564911282545</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>0.5</v>
       </c>
       <c r="B17" t="n">
-        <v>8717.227856540376</v>
+        <v>10041.54945581178</v>
       </c>
     </row>
     <row r="18">
@@ -578,7 +578,7 @@
         <v>0.5333333333333333</v>
       </c>
       <c r="B18" t="n">
-        <v>8889.082856292411</v>
+        <v>10237.32175682418</v>
       </c>
     </row>
     <row r="19">
@@ -586,7 +586,7 @@
         <v>0.5666666666666667</v>
       </c>
       <c r="B19" t="n">
-        <v>9100.810779565025</v>
+        <v>10480.38340354335</v>
       </c>
     </row>
     <row r="20">
@@ -594,7 +594,7 @@
         <v>0.6</v>
       </c>
       <c r="B20" t="n">
-        <v>9542.510798792076</v>
+        <v>10730.56883722468</v>
       </c>
     </row>
     <row r="21">
@@ -602,7 +602,7 @@
         <v>0.6333333333333333</v>
       </c>
       <c r="B21" t="n">
-        <v>9699.766527666708</v>
+        <v>10887.0411563089</v>
       </c>
     </row>
     <row r="22">
@@ -610,7 +610,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>9927.335242497451</v>
+        <v>11162.78405101858</v>
       </c>
     </row>
     <row r="23">
@@ -618,7 +618,7 @@
         <v>0.7</v>
       </c>
       <c r="B23" t="n">
-        <v>10080.73034756769</v>
+        <v>11285.41736594259</v>
       </c>
     </row>
     <row r="24">
@@ -626,7 +626,7 @@
         <v>0.7333333333333333</v>
       </c>
       <c r="B24" t="n">
-        <v>10379.20822118833</v>
+        <v>11585.38660893686</v>
       </c>
     </row>
     <row r="25">
@@ -634,7 +634,7 @@
         <v>0.7666666666666666</v>
       </c>
       <c r="B25" t="n">
-        <v>10567.4328674492</v>
+        <v>11687.4504678139</v>
       </c>
     </row>
     <row r="26">
@@ -642,7 +642,7 @@
         <v>0.8</v>
       </c>
       <c r="B26" t="n">
-        <v>10689.34202809058</v>
+        <v>11878.36887432134</v>
       </c>
     </row>
     <row r="27">
@@ -650,7 +650,7 @@
         <v>0.8333333333333334</v>
       </c>
       <c r="B27" t="n">
-        <v>10874.44348788996</v>
+        <v>12114.49714478112</v>
       </c>
     </row>
     <row r="28">
@@ -658,7 +658,7 @@
         <v>0.8666666666666667</v>
       </c>
       <c r="B28" t="n">
-        <v>10981.21679639662</v>
+        <v>12232.45668534909</v>
       </c>
     </row>
     <row r="29">
@@ -666,7 +666,7 @@
         <v>0.9</v>
       </c>
       <c r="B29" t="n">
-        <v>11193.3142242274</v>
+        <v>12336.5431969694</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +674,7 @@
         <v>0.9333333333333333</v>
       </c>
       <c r="B30" t="n">
-        <v>11323.58291949659</v>
+        <v>12528.32671445921</v>
       </c>
     </row>
     <row r="31">
@@ -682,7 +682,7 @@
         <v>0.9666666666666667</v>
       </c>
       <c r="B31" t="n">
-        <v>11468.94226962042</v>
+        <v>12638.49012198292</v>
       </c>
     </row>
     <row r="32">
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>11779.70520856214</v>
+        <v>12876.23976375084</v>
       </c>
     </row>
     <row r="33">
@@ -698,7 +698,7 @@
         <v>1.033333333333333</v>
       </c>
       <c r="B33" t="n">
-        <v>11864.82703546343</v>
+        <v>12994.18756820729</v>
       </c>
     </row>
     <row r="34">
@@ -706,7 +706,7 @@
         <v>1.066666666666667</v>
       </c>
       <c r="B34" t="n">
-        <v>12018.08718247714</v>
+        <v>13137.60954399211</v>
       </c>
     </row>
     <row r="35">
@@ -714,7 +714,7 @@
         <v>1.1</v>
       </c>
       <c r="B35" t="n">
-        <v>12172.32478077167</v>
+        <v>13387.23539579318</v>
       </c>
     </row>
     <row r="36">
@@ -722,7 +722,7 @@
         <v>1.133333333333333</v>
       </c>
       <c r="B36" t="n">
-        <v>12245.43284544658</v>
+        <v>13310.86209020602</v>
       </c>
     </row>
     <row r="37">
@@ -730,7 +730,7 @@
         <v>1.166666666666667</v>
       </c>
       <c r="B37" t="n">
-        <v>12325.09708835992</v>
+        <v>13534.82661666705</v>
       </c>
     </row>
     <row r="38">
@@ -738,7 +738,7 @@
         <v>1.2</v>
       </c>
       <c r="B38" t="n">
-        <v>12508.08077212547</v>
+        <v>13667.90292984921</v>
       </c>
     </row>
     <row r="39">
@@ -746,7 +746,7 @@
         <v>1.233333333333333</v>
       </c>
       <c r="B39" t="n">
-        <v>12635.42560401157</v>
+        <v>13802.71209478111</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +754,7 @@
         <v>1.266666666666667</v>
       </c>
       <c r="B40" t="n">
-        <v>12760.11872401384</v>
+        <v>13959.33622138699</v>
       </c>
     </row>
     <row r="41">
@@ -762,7 +762,7 @@
         <v>1.3</v>
       </c>
       <c r="B41" t="n">
-        <v>12848.50243680028</v>
+        <v>14032.85608012556</v>
       </c>
     </row>
     <row r="42">
@@ -770,7 +770,7 @@
         <v>1.333333333333333</v>
       </c>
       <c r="B42" t="n">
-        <v>12981.51286316499</v>
+        <v>14038.11226015806</v>
       </c>
     </row>
     <row r="43">
@@ -778,7 +778,7 @@
         <v>1.366666666666667</v>
       </c>
       <c r="B43" t="n">
-        <v>13054.52222273246</v>
+        <v>14098.93460621198</v>
       </c>
     </row>
     <row r="44">
@@ -786,7 +786,7 @@
         <v>1.4</v>
       </c>
       <c r="B44" t="n">
-        <v>13151.68102437822</v>
+        <v>14173.67659824644</v>
       </c>
     </row>
     <row r="45">
@@ -794,7 +794,7 @@
         <v>1.433333333333333</v>
       </c>
       <c r="B45" t="n">
-        <v>13287.58764252546</v>
+        <v>14278.4944349387</v>
       </c>
     </row>
     <row r="46">
@@ -802,7 +802,7 @@
         <v>1.466666666666667</v>
       </c>
       <c r="B46" t="n">
-        <v>13362.2976451646</v>
+        <v>14502.99238362768</v>
       </c>
     </row>
     <row r="47">
@@ -810,7 +810,7 @@
         <v>1.5</v>
       </c>
       <c r="B47" t="n">
-        <v>13490.48414440517</v>
+        <v>14794.52154245858</v>
       </c>
     </row>
     <row r="48">
@@ -818,7 +818,7 @@
         <v>1.533333333333333</v>
       </c>
       <c r="B48" t="n">
-        <v>13593.58868484142</v>
+        <v>14915.06365697691</v>
       </c>
     </row>
     <row r="49">
@@ -826,7 +826,7 @@
         <v>1.566666666666667</v>
       </c>
       <c r="B49" t="n">
-        <v>13596.94102936735</v>
+        <v>14947.84655382285</v>
       </c>
     </row>
     <row r="50">
@@ -834,7 +834,7 @@
         <v>1.6</v>
       </c>
       <c r="B50" t="n">
-        <v>13669.34852991616</v>
+        <v>15029.99038520521</v>
       </c>
     </row>
     <row r="51">
@@ -842,7 +842,7 @@
         <v>1.633333333333333</v>
       </c>
       <c r="B51" t="n">
-        <v>13776.84786942862</v>
+        <v>15134.43046697146</v>
       </c>
     </row>
     <row r="52">
@@ -850,7 +850,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="B52" t="n">
-        <v>13848.21150601052</v>
+        <v>15261.4251776523</v>
       </c>
     </row>
     <row r="53">
@@ -858,7 +858,7 @@
         <v>1.7</v>
       </c>
       <c r="B53" t="n">
-        <v>13919.58437113316</v>
+        <v>15316.65190593453</v>
       </c>
     </row>
     <row r="54">
@@ -866,7 +866,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="B54" t="n">
-        <v>13963.38835751431</v>
+        <v>15378.2451341638</v>
       </c>
     </row>
     <row r="55">
@@ -874,7 +874,7 @@
         <v>1.766666666666667</v>
       </c>
       <c r="B55" t="n">
-        <v>14110.50446643876</v>
+        <v>15502.70906282871</v>
       </c>
     </row>
     <row r="56">
@@ -882,7 +882,7 @@
         <v>1.8</v>
       </c>
       <c r="B56" t="n">
-        <v>14100.85439618242</v>
+        <v>15454.36020977322</v>
       </c>
     </row>
     <row r="57">
@@ -890,7 +890,7 @@
         <v>1.833333333333333</v>
       </c>
       <c r="B57" t="n">
-        <v>14189.26885625105</v>
+        <v>15570.32866329254</v>
       </c>
     </row>
     <row r="58">
@@ -898,7 +898,7 @@
         <v>1.866666666666667</v>
       </c>
       <c r="B58" t="n">
-        <v>14193.50717267355</v>
+        <v>15596.31859954413</v>
       </c>
     </row>
     <row r="59">
@@ -906,7 +906,7 @@
         <v>1.9</v>
       </c>
       <c r="B59" t="n">
-        <v>14238.93986774932</v>
+        <v>15606.31128178961</v>
       </c>
     </row>
     <row r="60">
@@ -914,7 +914,7 @@
         <v>1.933333333333333</v>
       </c>
       <c r="B60" t="n">
-        <v>14387.6725881826</v>
+        <v>15726.93835942123</v>
       </c>
     </row>
     <row r="61">
@@ -922,7 +922,7 @@
         <v>1.966666666666667</v>
       </c>
       <c r="B61" t="n">
-        <v>14394.71257736065</v>
+        <v>15739.24396771388</v>
       </c>
     </row>
     <row r="62">
@@ -930,7 +930,7 @@
         <v>2</v>
       </c>
       <c r="B62" t="n">
-        <v>14413.16179364517</v>
+        <v>15741.46777860923</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tested diff start point for ML model
</commit_message>
<xml_diff>
--- a/VisionModel/output/predicted_trajectoriesX.xlsx
+++ b/VisionModel/output/predicted_trajectoriesX.xlsx
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2896.016791289029</v>
+        <v>3921.658785588634</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>0.03333333333333333</v>
       </c>
       <c r="B3" t="n">
-        <v>3927.658649050765</v>
+        <v>4610.862094733957</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>0.06666666666666667</v>
       </c>
       <c r="B4" t="n">
-        <v>4534.029129713806</v>
+        <v>5293.444360066154</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>0.1</v>
       </c>
       <c r="B5" t="n">
-        <v>5421.269083827</v>
+        <v>5992.858100300337</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>0.1333333333333333</v>
       </c>
       <c r="B6" t="n">
-        <v>6030.559498840906</v>
+        <v>6648.827874564511</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>0.1666666666666667</v>
       </c>
       <c r="B7" t="n">
-        <v>6525.100025618548</v>
+        <v>7163.696237356986</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>0.2</v>
       </c>
       <c r="B8" t="n">
-        <v>6952.981220056842</v>
+        <v>7405.689504784748</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>0.2333333333333333</v>
       </c>
       <c r="B9" t="n">
-        <v>7484.473598119846</v>
+        <v>8165.13799976693</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>0.2666666666666667</v>
       </c>
       <c r="B10" t="n">
-        <v>7843.293491568781</v>
+        <v>8538.713075064825</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>0.3</v>
       </c>
       <c r="B11" t="n">
-        <v>8290.187337687727</v>
+        <v>9058.50130673449</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="B12" t="n">
-        <v>8685.730032810463</v>
+        <v>9336.660358264509</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>0.3666666666666666</v>
       </c>
       <c r="B13" t="n">
-        <v>9001.70057840767</v>
+        <v>9599.174680571881</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>0.4</v>
       </c>
       <c r="B14" t="n">
-        <v>9226.559212791988</v>
+        <v>10007.49005345957</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>0.4333333333333333</v>
       </c>
       <c r="B15" t="n">
-        <v>9552.597441704291</v>
+        <v>10321.62533764913</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>0.4666666666666667</v>
       </c>
       <c r="B16" t="n">
-        <v>9856.564911282545</v>
+        <v>10596.27984208827</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>0.5</v>
       </c>
       <c r="B17" t="n">
-        <v>10041.54945581178</v>
+        <v>10814.84726068009</v>
       </c>
     </row>
     <row r="18">
@@ -578,7 +578,7 @@
         <v>0.5333333333333333</v>
       </c>
       <c r="B18" t="n">
-        <v>10237.32175682418</v>
+        <v>11138.68398215823</v>
       </c>
     </row>
     <row r="19">
@@ -586,7 +586,7 @@
         <v>0.5666666666666667</v>
       </c>
       <c r="B19" t="n">
-        <v>10480.38340354335</v>
+        <v>11386.5604879413</v>
       </c>
     </row>
     <row r="20">
@@ -594,7 +594,7 @@
         <v>0.6</v>
       </c>
       <c r="B20" t="n">
-        <v>10730.56883722468</v>
+        <v>11296.02019712908</v>
       </c>
     </row>
     <row r="21">
@@ -602,7 +602,7 @@
         <v>0.6333333333333333</v>
       </c>
       <c r="B21" t="n">
-        <v>10887.0411563089</v>
+        <v>11482.99371222917</v>
       </c>
     </row>
     <row r="22">
@@ -610,7 +610,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>11162.78405101858</v>
+        <v>11676.5549147708</v>
       </c>
     </row>
     <row r="23">
@@ -618,7 +618,7 @@
         <v>0.7</v>
       </c>
       <c r="B23" t="n">
-        <v>11285.41736594259</v>
+        <v>11826.54117721885</v>
       </c>
     </row>
     <row r="24">
@@ -626,7 +626,7 @@
         <v>0.7333333333333333</v>
       </c>
       <c r="B24" t="n">
-        <v>11585.38660893686</v>
+        <v>12158.21408126541</v>
       </c>
     </row>
     <row r="25">
@@ -634,7 +634,7 @@
         <v>0.7666666666666666</v>
       </c>
       <c r="B25" t="n">
-        <v>11687.4504678139</v>
+        <v>12370.79548344</v>
       </c>
     </row>
     <row r="26">
@@ -642,7 +642,7 @@
         <v>0.8</v>
       </c>
       <c r="B26" t="n">
-        <v>11878.36887432134</v>
+        <v>12568.38345922562</v>
       </c>
     </row>
     <row r="27">
@@ -650,7 +650,7 @@
         <v>0.8333333333333334</v>
       </c>
       <c r="B27" t="n">
-        <v>12114.49714478112</v>
+        <v>12701.27060576151</v>
       </c>
     </row>
     <row r="28">
@@ -658,7 +658,7 @@
         <v>0.8666666666666667</v>
       </c>
       <c r="B28" t="n">
-        <v>12232.45668534909</v>
+        <v>12764.90919545843</v>
       </c>
     </row>
     <row r="29">
@@ -666,7 +666,7 @@
         <v>0.9</v>
       </c>
       <c r="B29" t="n">
-        <v>12336.5431969694</v>
+        <v>12907.95048228432</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +674,7 @@
         <v>0.9333333333333333</v>
       </c>
       <c r="B30" t="n">
-        <v>12528.32671445921</v>
+        <v>13084.51181512031</v>
       </c>
     </row>
     <row r="31">
@@ -682,7 +682,7 @@
         <v>0.9666666666666667</v>
       </c>
       <c r="B31" t="n">
-        <v>12638.49012198292</v>
+        <v>13243.12588675456</v>
       </c>
     </row>
     <row r="32">
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>12876.23976375084</v>
+        <v>13576.59158557177</v>
       </c>
     </row>
     <row r="33">
@@ -698,7 +698,7 @@
         <v>1.033333333333333</v>
       </c>
       <c r="B33" t="n">
-        <v>12994.18756820729</v>
+        <v>13669.3144584906</v>
       </c>
     </row>
     <row r="34">
@@ -706,7 +706,7 @@
         <v>1.066666666666667</v>
       </c>
       <c r="B34" t="n">
-        <v>13137.60954399211</v>
+        <v>13878.21174268121</v>
       </c>
     </row>
     <row r="35">
@@ -714,7 +714,7 @@
         <v>1.1</v>
       </c>
       <c r="B35" t="n">
-        <v>13387.23539579318</v>
+        <v>14047.12327388834</v>
       </c>
     </row>
     <row r="36">
@@ -722,7 +722,7 @@
         <v>1.133333333333333</v>
       </c>
       <c r="B36" t="n">
-        <v>13310.86209020602</v>
+        <v>14152.66769723202</v>
       </c>
     </row>
     <row r="37">
@@ -730,7 +730,7 @@
         <v>1.166666666666667</v>
       </c>
       <c r="B37" t="n">
-        <v>13534.82661666705</v>
+        <v>14271.97539074888</v>
       </c>
     </row>
     <row r="38">
@@ -738,7 +738,7 @@
         <v>1.2</v>
       </c>
       <c r="B38" t="n">
-        <v>13667.90292984921</v>
+        <v>14434.42331817191</v>
       </c>
     </row>
     <row r="39">
@@ -746,7 +746,7 @@
         <v>1.233333333333333</v>
       </c>
       <c r="B39" t="n">
-        <v>13802.71209478111</v>
+        <v>14479.19064378691</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +754,7 @@
         <v>1.266666666666667</v>
       </c>
       <c r="B40" t="n">
-        <v>13959.33622138699</v>
+        <v>14668.98115302313</v>
       </c>
     </row>
     <row r="41">
@@ -762,7 +762,7 @@
         <v>1.3</v>
       </c>
       <c r="B41" t="n">
-        <v>14032.85608012556</v>
+        <v>14764.03071671831</v>
       </c>
     </row>
     <row r="42">
@@ -770,7 +770,7 @@
         <v>1.333333333333333</v>
       </c>
       <c r="B42" t="n">
-        <v>14038.11226015806</v>
+        <v>14885.69482890222</v>
       </c>
     </row>
     <row r="43">
@@ -778,7 +778,7 @@
         <v>1.366666666666667</v>
       </c>
       <c r="B43" t="n">
-        <v>14098.93460621198</v>
+        <v>14980.07477207137</v>
       </c>
     </row>
     <row r="44">
@@ -786,7 +786,7 @@
         <v>1.4</v>
       </c>
       <c r="B44" t="n">
-        <v>14173.67659824644</v>
+        <v>14934.35330678715</v>
       </c>
     </row>
     <row r="45">
@@ -794,7 +794,7 @@
         <v>1.433333333333333</v>
       </c>
       <c r="B45" t="n">
-        <v>14278.4944349387</v>
+        <v>15071.79478457906</v>
       </c>
     </row>
     <row r="46">
@@ -802,7 +802,7 @@
         <v>1.466666666666667</v>
       </c>
       <c r="B46" t="n">
-        <v>14502.99238362768</v>
+        <v>15132.62758229976</v>
       </c>
     </row>
     <row r="47">
@@ -810,7 +810,7 @@
         <v>1.5</v>
       </c>
       <c r="B47" t="n">
-        <v>14794.52154245858</v>
+        <v>15233.73239740377</v>
       </c>
     </row>
     <row r="48">
@@ -818,7 +818,7 @@
         <v>1.533333333333333</v>
       </c>
       <c r="B48" t="n">
-        <v>14915.06365697691</v>
+        <v>15372.4660136289</v>
       </c>
     </row>
     <row r="49">
@@ -826,7 +826,7 @@
         <v>1.566666666666667</v>
       </c>
       <c r="B49" t="n">
-        <v>14947.84655382285</v>
+        <v>15369.68032229482</v>
       </c>
     </row>
     <row r="50">
@@ -834,7 +834,7 @@
         <v>1.6</v>
       </c>
       <c r="B50" t="n">
-        <v>15029.99038520521</v>
+        <v>15407.38825627885</v>
       </c>
     </row>
     <row r="51">
@@ -842,7 +842,7 @@
         <v>1.633333333333333</v>
       </c>
       <c r="B51" t="n">
-        <v>15134.43046697146</v>
+        <v>15536.51856861041</v>
       </c>
     </row>
     <row r="52">
@@ -850,7 +850,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="B52" t="n">
-        <v>15261.4251776523</v>
+        <v>15558.20613624086</v>
       </c>
     </row>
     <row r="53">
@@ -858,7 +858,7 @@
         <v>1.7</v>
       </c>
       <c r="B53" t="n">
-        <v>15316.65190593453</v>
+        <v>15675.38133453084</v>
       </c>
     </row>
     <row r="54">
@@ -866,7 +866,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="B54" t="n">
-        <v>15378.2451341638</v>
+        <v>15721.38662937669</v>
       </c>
     </row>
     <row r="55">
@@ -874,7 +874,7 @@
         <v>1.766666666666667</v>
       </c>
       <c r="B55" t="n">
-        <v>15502.70906282871</v>
+        <v>15893.93215097395</v>
       </c>
     </row>
     <row r="56">
@@ -882,7 +882,7 @@
         <v>1.8</v>
       </c>
       <c r="B56" t="n">
-        <v>15454.36020977322</v>
+        <v>15831.68663770271</v>
       </c>
     </row>
     <row r="57">
@@ -890,7 +890,7 @@
         <v>1.833333333333333</v>
       </c>
       <c r="B57" t="n">
-        <v>15570.32866329254</v>
+        <v>15951.09853415263</v>
       </c>
     </row>
     <row r="58">
@@ -898,7 +898,7 @@
         <v>1.866666666666667</v>
       </c>
       <c r="B58" t="n">
-        <v>15596.31859954413</v>
+        <v>15960.4713648951</v>
       </c>
     </row>
     <row r="59">
@@ -906,7 +906,7 @@
         <v>1.9</v>
       </c>
       <c r="B59" t="n">
-        <v>15606.31128178961</v>
+        <v>15905.0524474193</v>
       </c>
     </row>
     <row r="60">
@@ -914,7 +914,7 @@
         <v>1.933333333333333</v>
       </c>
       <c r="B60" t="n">
-        <v>15726.93835942123</v>
+        <v>16036.57893001658</v>
       </c>
     </row>
     <row r="61">
@@ -922,7 +922,7 @@
         <v>1.966666666666667</v>
       </c>
       <c r="B61" t="n">
-        <v>15739.24396771388</v>
+        <v>16050.71011181273</v>
       </c>
     </row>
     <row r="62">
@@ -930,7 +930,7 @@
         <v>2</v>
       </c>
       <c r="B62" t="n">
-        <v>15741.46777860923</v>
+        <v>16220.6029797299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
combined prediction code into single class and added code to log timings for different operations
</commit_message>
<xml_diff>
--- a/VisionModel/output/predicted_trajectoriesX.xlsx
+++ b/VisionModel/output/predicted_trajectoriesX.xlsx
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>3921.658785588634</v>
+        <v>4294.964340500327</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>0.03333333333333333</v>
       </c>
       <c r="B3" t="n">
-        <v>4610.862094733957</v>
+        <v>4926.153965455343</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>0.06666666666666667</v>
       </c>
       <c r="B4" t="n">
-        <v>5293.444360066154</v>
+        <v>5464.408501268852</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>0.1</v>
       </c>
       <c r="B5" t="n">
-        <v>5992.858100300337</v>
+        <v>6056.764868294075</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>0.1333333333333333</v>
       </c>
       <c r="B6" t="n">
-        <v>6648.827874564511</v>
+        <v>6833.226149065153</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>0.1666666666666667</v>
       </c>
       <c r="B7" t="n">
-        <v>7163.696237356986</v>
+        <v>7358.258706741193</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>0.2</v>
       </c>
       <c r="B8" t="n">
-        <v>7405.689504784748</v>
+        <v>7560.823388780289</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>0.2333333333333333</v>
       </c>
       <c r="B9" t="n">
-        <v>8165.13799976693</v>
+        <v>8156.464403688821</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>0.2666666666666667</v>
       </c>
       <c r="B10" t="n">
-        <v>8538.713075064825</v>
+        <v>8490.618780374585</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>0.3</v>
       </c>
       <c r="B11" t="n">
-        <v>9058.50130673449</v>
+        <v>9083.484782114929</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="B12" t="n">
-        <v>9336.660358264509</v>
+        <v>9313.896030017604</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>0.3666666666666666</v>
       </c>
       <c r="B13" t="n">
-        <v>9599.174680571881</v>
+        <v>9502.365027749456</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>0.4</v>
       </c>
       <c r="B14" t="n">
-        <v>10007.49005345957</v>
+        <v>9991.299151908721</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>0.4333333333333333</v>
       </c>
       <c r="B15" t="n">
-        <v>10321.62533764913</v>
+        <v>10287.82191723134</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>0.4666666666666667</v>
       </c>
       <c r="B16" t="n">
-        <v>10596.27984208827</v>
+        <v>10617.72211794718</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>0.5</v>
       </c>
       <c r="B17" t="n">
-        <v>10814.84726068009</v>
+        <v>10806.93903147523</v>
       </c>
     </row>
     <row r="18">
@@ -578,7 +578,7 @@
         <v>0.5333333333333333</v>
       </c>
       <c r="B18" t="n">
-        <v>11138.68398215823</v>
+        <v>11076.81108858635</v>
       </c>
     </row>
     <row r="19">
@@ -586,7 +586,7 @@
         <v>0.5666666666666667</v>
       </c>
       <c r="B19" t="n">
-        <v>11386.5604879413</v>
+        <v>11301.06367270383</v>
       </c>
     </row>
     <row r="20">
@@ -594,7 +594,7 @@
         <v>0.6</v>
       </c>
       <c r="B20" t="n">
-        <v>11296.02019712908</v>
+        <v>11618.31939991226</v>
       </c>
     </row>
     <row r="21">
@@ -602,7 +602,7 @@
         <v>0.6333333333333333</v>
       </c>
       <c r="B21" t="n">
-        <v>11482.99371222917</v>
+        <v>11765.0961080947</v>
       </c>
     </row>
     <row r="22">
@@ -610,7 +610,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>11676.5549147708</v>
+        <v>11894.41129315888</v>
       </c>
     </row>
     <row r="23">
@@ -618,7 +618,7 @@
         <v>0.7</v>
       </c>
       <c r="B23" t="n">
-        <v>11826.54117721885</v>
+        <v>11968.66750596234</v>
       </c>
     </row>
     <row r="24">
@@ -626,7 +626,7 @@
         <v>0.7333333333333333</v>
       </c>
       <c r="B24" t="n">
-        <v>12158.21408126541</v>
+        <v>12198.39333331799</v>
       </c>
     </row>
     <row r="25">
@@ -634,7 +634,7 @@
         <v>0.7666666666666666</v>
       </c>
       <c r="B25" t="n">
-        <v>12370.79548344</v>
+        <v>12444.63308485151</v>
       </c>
     </row>
     <row r="26">
@@ -642,7 +642,7 @@
         <v>0.8</v>
       </c>
       <c r="B26" t="n">
-        <v>12568.38345922562</v>
+        <v>12739.27831815544</v>
       </c>
     </row>
     <row r="27">
@@ -650,7 +650,7 @@
         <v>0.8333333333333334</v>
       </c>
       <c r="B27" t="n">
-        <v>12701.27060576151</v>
+        <v>12834.92636584731</v>
       </c>
     </row>
     <row r="28">
@@ -658,7 +658,7 @@
         <v>0.8666666666666667</v>
       </c>
       <c r="B28" t="n">
-        <v>12764.90919545843</v>
+        <v>13039.99433250989</v>
       </c>
     </row>
     <row r="29">
@@ -666,7 +666,7 @@
         <v>0.9</v>
       </c>
       <c r="B29" t="n">
-        <v>12907.95048228432</v>
+        <v>13210.43681948788</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +674,7 @@
         <v>0.9333333333333333</v>
       </c>
       <c r="B30" t="n">
-        <v>13084.51181512031</v>
+        <v>13355.84276198929</v>
       </c>
     </row>
     <row r="31">
@@ -682,7 +682,7 @@
         <v>0.9666666666666667</v>
       </c>
       <c r="B31" t="n">
-        <v>13243.12588675456</v>
+        <v>13478.52368072836</v>
       </c>
     </row>
     <row r="32">
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>13576.59158557177</v>
+        <v>13679.00729914817</v>
       </c>
     </row>
     <row r="33">
@@ -698,7 +698,7 @@
         <v>1.033333333333333</v>
       </c>
       <c r="B33" t="n">
-        <v>13669.3144584906</v>
+        <v>13752.45818072856</v>
       </c>
     </row>
     <row r="34">
@@ -706,7 +706,7 @@
         <v>1.066666666666667</v>
       </c>
       <c r="B34" t="n">
-        <v>13878.21174268121</v>
+        <v>13979.6642935727</v>
       </c>
     </row>
     <row r="35">
@@ -714,7 +714,7 @@
         <v>1.1</v>
       </c>
       <c r="B35" t="n">
-        <v>14047.12327388834</v>
+        <v>14107.25641726138</v>
       </c>
     </row>
     <row r="36">
@@ -722,7 +722,7 @@
         <v>1.133333333333333</v>
       </c>
       <c r="B36" t="n">
-        <v>14152.66769723202</v>
+        <v>13958.81434771256</v>
       </c>
     </row>
     <row r="37">
@@ -730,7 +730,7 @@
         <v>1.166666666666667</v>
       </c>
       <c r="B37" t="n">
-        <v>14271.97539074888</v>
+        <v>14079.94621813633</v>
       </c>
     </row>
     <row r="38">
@@ -738,7 +738,7 @@
         <v>1.2</v>
       </c>
       <c r="B38" t="n">
-        <v>14434.42331817191</v>
+        <v>14240.6376546265</v>
       </c>
     </row>
     <row r="39">
@@ -746,7 +746,7 @@
         <v>1.233333333333333</v>
       </c>
       <c r="B39" t="n">
-        <v>14479.19064378691</v>
+        <v>14317.23417890966</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +754,7 @@
         <v>1.266666666666667</v>
       </c>
       <c r="B40" t="n">
-        <v>14668.98115302313</v>
+        <v>14488.99035059528</v>
       </c>
     </row>
     <row r="41">
@@ -762,7 +762,7 @@
         <v>1.3</v>
       </c>
       <c r="B41" t="n">
-        <v>14764.03071671831</v>
+        <v>14578.97998375641</v>
       </c>
     </row>
     <row r="42">
@@ -770,7 +770,7 @@
         <v>1.333333333333333</v>
       </c>
       <c r="B42" t="n">
-        <v>14885.69482890222</v>
+        <v>14722.45546914963</v>
       </c>
     </row>
     <row r="43">
@@ -778,7 +778,7 @@
         <v>1.366666666666667</v>
       </c>
       <c r="B43" t="n">
-        <v>14980.07477207137</v>
+        <v>14805.14108839904</v>
       </c>
     </row>
     <row r="44">
@@ -786,7 +786,7 @@
         <v>1.4</v>
       </c>
       <c r="B44" t="n">
-        <v>14934.35330678715</v>
+        <v>14884.05182910904</v>
       </c>
     </row>
     <row r="45">
@@ -794,7 +794,7 @@
         <v>1.433333333333333</v>
       </c>
       <c r="B45" t="n">
-        <v>15071.79478457906</v>
+        <v>15238.22996678246</v>
       </c>
     </row>
     <row r="46">
@@ -802,7 +802,7 @@
         <v>1.466666666666667</v>
       </c>
       <c r="B46" t="n">
-        <v>15132.62758229976</v>
+        <v>15297.92464207829</v>
       </c>
     </row>
     <row r="47">
@@ -810,7 +810,7 @@
         <v>1.5</v>
       </c>
       <c r="B47" t="n">
-        <v>15233.73239740377</v>
+        <v>15403.49262767791</v>
       </c>
     </row>
     <row r="48">
@@ -818,7 +818,7 @@
         <v>1.533333333333333</v>
       </c>
       <c r="B48" t="n">
-        <v>15372.4660136289</v>
+        <v>15576.79312480013</v>
       </c>
     </row>
     <row r="49">
@@ -826,7 +826,7 @@
         <v>1.566666666666667</v>
       </c>
       <c r="B49" t="n">
-        <v>15369.68032229482</v>
+        <v>15561.50801447334</v>
       </c>
     </row>
     <row r="50">
@@ -834,7 +834,7 @@
         <v>1.6</v>
       </c>
       <c r="B50" t="n">
-        <v>15407.38825627885</v>
+        <v>15575.54402581014</v>
       </c>
     </row>
     <row r="51">
@@ -842,7 +842,7 @@
         <v>1.633333333333333</v>
       </c>
       <c r="B51" t="n">
-        <v>15536.51856861041</v>
+        <v>15695.4091117376</v>
       </c>
     </row>
     <row r="52">
@@ -850,7 +850,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="B52" t="n">
-        <v>15558.20613624086</v>
+        <v>15709.20306581252</v>
       </c>
     </row>
     <row r="53">
@@ -858,7 +858,7 @@
         <v>1.7</v>
       </c>
       <c r="B53" t="n">
-        <v>15675.38133453084</v>
+        <v>15831.61629122414</v>
       </c>
     </row>
     <row r="54">
@@ -866,7 +866,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="B54" t="n">
-        <v>15721.38662937669</v>
+        <v>15853.93741127316</v>
       </c>
     </row>
     <row r="55">
@@ -874,7 +874,7 @@
         <v>1.766666666666667</v>
       </c>
       <c r="B55" t="n">
-        <v>15893.93215097395</v>
+        <v>16047.25741812299</v>
       </c>
     </row>
     <row r="56">
@@ -882,7 +882,7 @@
         <v>1.8</v>
       </c>
       <c r="B56" t="n">
-        <v>15831.68663770271</v>
+        <v>15934.67028225771</v>
       </c>
     </row>
     <row r="57">
@@ -890,7 +890,7 @@
         <v>1.833333333333333</v>
       </c>
       <c r="B57" t="n">
-        <v>15951.09853415263</v>
+        <v>16091.04934136898</v>
       </c>
     </row>
     <row r="58">
@@ -898,7 +898,7 @@
         <v>1.866666666666667</v>
       </c>
       <c r="B58" t="n">
-        <v>15960.4713648951</v>
+        <v>16094.30334947824</v>
       </c>
     </row>
     <row r="59">
@@ -906,7 +906,7 @@
         <v>1.9</v>
       </c>
       <c r="B59" t="n">
-        <v>15905.0524474193</v>
+        <v>15966.86512221618</v>
       </c>
     </row>
     <row r="60">
@@ -914,7 +914,7 @@
         <v>1.933333333333333</v>
       </c>
       <c r="B60" t="n">
-        <v>16036.57893001658</v>
+        <v>16060.77889280614</v>
       </c>
     </row>
     <row r="61">
@@ -922,7 +922,7 @@
         <v>1.966666666666667</v>
       </c>
       <c r="B61" t="n">
-        <v>16050.71011181273</v>
+        <v>16081.81664056357</v>
       </c>
     </row>
     <row r="62">
@@ -930,7 +930,7 @@
         <v>2</v>
       </c>
       <c r="B62" t="n">
-        <v>16220.6029797299</v>
+        <v>16136.94882170101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>